<commit_message>
SON24 new content: Charts and tables: DR42 Level of trust, fairness and helpfulness: Re-do because of data errors
</commit_message>
<xml_diff>
--- a/son/content/drivers_of_social_mobility/social_capital_and_connections/level_of_trust,_fairness_and_helpfulness/2.0/DR42-2.0-level-of-trust-fairness-and-helpfulness--by-year--table-format.xlsx
+++ b/son/content/drivers_of_social_mobility/social_capital_and_connections/level_of_trust,_fairness_and_helpfulness/2.0/DR42-2.0-level-of-trust-fairness-and-helpfulness--by-year--table-format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Government Equality Hub\SON23\Code\smc-son\son\content\drivers_of_social_mobility\social_capital_and_connections\level_of_trust,_fairness_and_helpfulness\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{357DF61A-8A82-42B0-A325-C1CF450F8155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1950BE9A-5C62-4778-BD23-5C978612F623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18000" xr2:uid="{C44A1148-5522-4C6E-AE50-9F086811560C}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -678,7 +678,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="james" refreshedDate="45482.993294560183" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="31" xr:uid="{38E71F29-DABD-4D09-8F06-57355DE5345D}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="james" refreshedDate="45488.530816550927" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="31" xr:uid="{38E71F29-DABD-4D09-8F06-57355DE5345D}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:T1048576" sheet="DR42-level-of-trust-fairness-an"/>
   </cacheSource>
@@ -740,19 +740,19 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="value" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5.3431754874651798" maxValue="6.0917516218721"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5.0473401659346004" maxValue="5.93554006968641"/>
     </cacheField>
     <cacheField name="sample_size" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1079" maxValue="2293"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1149" maxValue="2422"/>
     </cacheField>
     <cacheField name="lci" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5.2520507928693698" maxValue="5.9830158548003602"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="4.9513657917123899" maxValue="5.8360152588950802"/>
     </cacheField>
     <cacheField name="uci" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5.4301682870641796" maxValue="6.2004873889438503"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5.1433145401568199" maxValue="6.0523788702590098"/>
     </cacheField>
     <cacheField name="se" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="3.8245848110437297E-2" maxValue="5.8214758734013501E-2"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="3.9211125303035201E-2" maxValue="6.5579958259253002E-2"/>
     </cacheField>
     <cacheField name="unit" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -785,11 +785,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.7406824146981599"/>
-    <n v="1905"/>
-    <n v="5.6559052779569496"/>
-    <n v="5.8254595514393799"/>
-    <n v="4.3253641194496303E-2"/>
+    <n v="5.5454545454545396"/>
+    <n v="2052"/>
+    <n v="5.4538150077266403"/>
+    <n v="5.6370940831824496"/>
+    <n v="4.6754866187707002E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -807,11 +807,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.58215223097113"/>
-    <n v="1905"/>
-    <n v="5.4966319114219697"/>
-    <n v="5.6676725505202903"/>
-    <n v="4.3632816096509597E-2"/>
+    <n v="5.4247311827956999"/>
+    <n v="2052"/>
+    <n v="5.3347518310843096"/>
+    <n v="5.5147105345070901"/>
+    <n v="4.5907832505811798E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -829,11 +829,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.34383202099737"/>
-    <n v="1905"/>
-    <n v="5.2574957549305603"/>
-    <n v="5.4301682870641796"/>
-    <n v="4.4049115340209499E-2"/>
+    <n v="5.0473401659346004"/>
+    <n v="2052"/>
+    <n v="4.9513657917123899"/>
+    <n v="5.1433145401568199"/>
+    <n v="4.8966517460314198E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -851,11 +851,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.6607242339832897"/>
-    <n v="1795"/>
-    <n v="5.5716533236806498"/>
-    <n v="5.7497951442859296"/>
-    <n v="4.5444341991142799E-2"/>
+    <n v="5.5459373340414198"/>
+    <n v="1897"/>
+    <n v="5.4532914123852203"/>
+    <n v="5.6385832556976201"/>
+    <n v="4.72683273756122E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -873,11 +873,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.7615598885793897"/>
-    <n v="1795"/>
-    <n v="5.6733938316469201"/>
-    <n v="5.8497259455118602"/>
-    <n v="4.4982682108403303E-2"/>
+    <n v="5.6663135593220399"/>
+    <n v="1897"/>
+    <n v="5.5748344607409903"/>
+    <n v="5.7577926579030798"/>
+    <n v="4.6673009480124102E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -895,11 +895,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.3431754874651798"/>
-    <n v="1795"/>
-    <n v="5.2520507928693698"/>
-    <n v="5.4343001820609897"/>
-    <n v="4.64921911203105E-2"/>
+    <n v="5.1362916006339203"/>
+    <n v="1897"/>
+    <n v="5.0381822965655099"/>
+    <n v="5.2344009047023201"/>
+    <n v="5.0055767381839103E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -917,11 +917,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.9067609368095404"/>
-    <n v="2263"/>
-    <n v="5.8290963025940004"/>
-    <n v="5.9844255710250804"/>
-    <n v="3.9624813375276097E-2"/>
+    <n v="5.7802013422818801"/>
+    <n v="2394"/>
+    <n v="5.6976388389597199"/>
+    <n v="5.8627638456040296"/>
+    <n v="4.2123726184772801E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -939,11 +939,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.80247459125055"/>
-    <n v="2263"/>
-    <n v="5.7248129546277404"/>
-    <n v="5.8801362278733604"/>
-    <n v="3.9623283991231301E-2"/>
+    <n v="5.6838574423480104"/>
+    <n v="2394"/>
+    <n v="5.6025661233647099"/>
+    <n v="5.7651487613313099"/>
+    <n v="4.1475162746580502E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -961,11 +961,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.6009721608484302"/>
-    <n v="2263"/>
-    <n v="5.5203799726219502"/>
-    <n v="5.6815643490749199"/>
-    <n v="4.1118463380859102E-2"/>
+    <n v="5.4035234899328799"/>
+    <n v="2394"/>
+    <n v="5.31647088441989"/>
+    <n v="5.4905760954458698"/>
+    <n v="4.4414594649484697E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -983,11 +983,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.8304014433919704"/>
-    <n v="2217"/>
-    <n v="5.7496546459367499"/>
-    <n v="5.91114824084719"/>
-    <n v="4.11973456404175E-2"/>
+    <n v="5.6821870995301103"/>
+    <n v="2352"/>
+    <n v="5.5965545601090598"/>
+    <n v="5.7678196389511696"/>
+    <n v="4.3690071133192801E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1005,11 +1005,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.7365809652683799"/>
-    <n v="2217"/>
-    <n v="5.6560866722530099"/>
-    <n v="5.8170752582837499"/>
-    <n v="4.1068516844576103E-2"/>
+    <n v="5.62079250106519"/>
+    <n v="2352"/>
+    <n v="5.5368182596788103"/>
+    <n v="5.7047667424515698"/>
+    <n v="4.2844000707334601E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1027,11 +1027,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.5002255299954896"/>
-    <n v="2217"/>
-    <n v="5.4167830858875199"/>
-    <n v="5.5836679741034603"/>
-    <n v="4.2572675565291603E-2"/>
+    <n v="5.2687393526405497"/>
+    <n v="2352"/>
+    <n v="5.1779302226919004"/>
+    <n v="5.3595484825891901"/>
+    <n v="4.6331188749307799E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1049,11 +1049,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.7025730484082002"/>
-    <n v="2293"/>
-    <n v="5.6236329116104997"/>
-    <n v="5.7815131852058999"/>
-    <n v="4.0275579998826597E-2"/>
+    <n v="5.6193656093489102"/>
+    <n v="2422"/>
+    <n v="5.5378847815901899"/>
+    <n v="5.7008464371076402"/>
+    <n v="4.1571850897309297E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1071,11 +1071,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.8791975577845603"/>
-    <n v="2293"/>
-    <n v="5.8042356954881003"/>
-    <n v="5.9541594200810204"/>
-    <n v="3.8245848110437297E-2"/>
+    <n v="5.7862785862785904"/>
+    <n v="2422"/>
+    <n v="5.7094247806846399"/>
+    <n v="5.86313239187254"/>
+    <n v="3.9211125303035201E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1093,11 +1093,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.5307457479284796"/>
-    <n v="2293"/>
-    <n v="5.4503016860928799"/>
-    <n v="5.6111898097640696"/>
-    <n v="4.1042888691630502E-2"/>
+    <n v="5.3556935817805398"/>
+    <n v="2422"/>
+    <n v="5.2694984210147604"/>
+    <n v="5.44188874254632"/>
+    <n v="4.3977122839684697E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1115,11 +1115,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.8761425959780604"/>
-    <n v="2188"/>
-    <n v="5.7992877551457704"/>
-    <n v="5.9529974368103602"/>
-    <n v="3.9211653485864702E-2"/>
+    <n v="5.7861552028218703"/>
+    <n v="2286"/>
+    <n v="5.70667760163722"/>
+    <n v="5.8656328040065198"/>
+    <n v="4.05497965227802E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1137,11 +1137,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.8976234003656298"/>
-    <n v="2188"/>
-    <n v="5.8197122561245198"/>
-    <n v="5.9755345446067398"/>
-    <n v="3.9750583796483697E-2"/>
+    <n v="5.8337730870712399"/>
+    <n v="2286"/>
+    <n v="5.7540942154058703"/>
+    <n v="5.9134519587366103"/>
+    <n v="4.06524855435558E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1159,11 +1159,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.5086837294332698"/>
-    <n v="2188"/>
-    <n v="5.4266479176051403"/>
-    <n v="5.5907195412614001"/>
-    <n v="4.1855006034758897E-2"/>
+    <n v="5.3862038664323402"/>
+    <n v="2286"/>
+    <n v="5.2996685740229799"/>
+    <n v="5.4727391588416898"/>
+    <n v="4.4150659392529802E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1181,11 +1181,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="6.0089495996231799"/>
-    <n v="2123"/>
-    <n v="5.93104704865216"/>
-    <n v="6.0868521505941899"/>
-    <n v="3.9746199475006003E-2"/>
+    <n v="5.8399822695035501"/>
+    <n v="2264"/>
+    <n v="5.7552859176087496"/>
+    <n v="5.92467862139834"/>
+    <n v="4.3212424436121603E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1203,11 +1203,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="6.06029203956665"/>
-    <n v="2123"/>
-    <n v="5.9802970151463501"/>
-    <n v="6.1402870639869498"/>
-    <n v="4.0813787969540299E-2"/>
+    <n v="5.9203539823008899"/>
+    <n v="2264"/>
+    <n v="5.8360152588950802"/>
+    <n v="6.0046927057066899"/>
+    <n v="4.3029960921327E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1225,11 +1225,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.6288271314177996"/>
-    <n v="2123"/>
-    <n v="5.5466383520923497"/>
-    <n v="5.7110159107432601"/>
-    <n v="4.1933050676253601E-2"/>
+    <n v="5.3756637168141603"/>
+    <n v="2264"/>
+    <n v="5.2842870703895501"/>
+    <n v="5.4670403632387696"/>
+    <n v="4.6620737971741003E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1247,11 +1247,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.9224890829694301"/>
-    <n v="1832"/>
-    <n v="5.8381770020975301"/>
-    <n v="6.0068011638413301"/>
-    <n v="4.30163677917847E-2"/>
+    <n v="5.7407975460122698"/>
+    <n v="1959"/>
+    <n v="5.6495557880663902"/>
+    <n v="5.8320393039581502"/>
+    <n v="4.6551917319327597E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1269,11 +1269,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.9432314410480398"/>
-    <n v="1832"/>
-    <n v="5.8606825670878102"/>
-    <n v="6.0257803150082596"/>
-    <n v="4.21167724286838E-2"/>
+    <n v="5.8065506653019403"/>
+    <n v="1959"/>
+    <n v="5.7193733618865803"/>
+    <n v="5.8937279687173101"/>
+    <n v="4.4478216028247503E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1291,11 +1291,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.5911572052401803"/>
-    <n v="1832"/>
-    <n v="5.5032685227715197"/>
-    <n v="5.6790458877088303"/>
-    <n v="4.4841164524824798E-2"/>
+    <n v="5.3244762391415401"/>
+    <n v="1959"/>
+    <n v="5.2266838881319799"/>
+    <n v="5.4222685901511003"/>
+    <n v="4.9894056637532103E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1313,11 +1313,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.9404587603709098"/>
-    <n v="2049"/>
-    <n v="5.8585603661495202"/>
-    <n v="6.0223571545923003"/>
-    <n v="4.1784895010913002E-2"/>
+    <n v="5.7492020063839497"/>
+    <n v="2204"/>
+    <n v="5.6617764785955096"/>
+    <n v="5.8366275341723899"/>
+    <n v="4.4604861116550799E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1335,11 +1335,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.9321620302586604"/>
-    <n v="2049"/>
-    <n v="5.8511807037635899"/>
-    <n v="6.01314335675373"/>
-    <n v="4.13170033138116E-2"/>
+    <n v="5.7752502274795301"/>
+    <n v="2204"/>
+    <n v="5.69047387146838"/>
+    <n v="5.8600265834906802"/>
+    <n v="4.3253242862831401E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1357,11 +1357,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.4543679843826203"/>
-    <n v="2049"/>
-    <n v="5.3673362899802397"/>
-    <n v="5.5413996787850097"/>
-    <n v="4.44039257155045E-2"/>
+    <n v="5.17507958162801"/>
+    <n v="2204"/>
+    <n v="5.0795520173124897"/>
+    <n v="5.2706071459435302"/>
+    <n v="4.8738553222203801E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1379,11 +1379,11 @@
     <x v="0"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="6.0917516218721"/>
-    <n v="1079"/>
-    <n v="5.9830158548003602"/>
-    <n v="6.2004873889438503"/>
-    <n v="5.5477432179461598E-2"/>
+    <n v="5.9128160418483002"/>
+    <n v="1149"/>
+    <n v="5.7944868591251799"/>
+    <n v="6.0311452245714197"/>
+    <n v="6.0372032001593197E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1401,11 +1401,11 @@
     <x v="1"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="6.03985171455051"/>
-    <n v="1079"/>
-    <n v="5.9279814454395598"/>
-    <n v="6.1517219836614601"/>
-    <n v="5.7076667913752502E-2"/>
+    <n v="5.93554006968641"/>
+    <n v="1149"/>
+    <n v="5.8187012691138102"/>
+    <n v="6.0523788702590098"/>
+    <n v="5.96116329452024E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1423,11 +1423,11 @@
     <x v="2"/>
     <s v="NA"/>
     <s v="NA"/>
-    <n v="5.7015755329008302"/>
-    <n v="1079"/>
-    <n v="5.5874746057821696"/>
-    <n v="5.8156764600194997"/>
-    <n v="5.8214758734013501E-2"/>
+    <n v="5.4255874673629201"/>
+    <n v="1149"/>
+    <n v="5.2970507491747902"/>
+    <n v="5.5541241855510597"/>
+    <n v="6.5579958259253002E-2"/>
     <s v="Mean"/>
     <s v="NA"/>
   </r>
@@ -1457,7 +1457,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{06A69CC7-B7E0-4699-8206-99BCE5D96459}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{06A69CC7-B7E0-4699-8206-99BCE5D96459}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Year">
   <location ref="A3:D14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -1934,13 +1934,13 @@
         <v>2020</v>
       </c>
       <c r="B5" s="3">
-        <v>5.7015755329008302</v>
+        <v>5.4255874673629201</v>
       </c>
       <c r="C5" s="3">
-        <v>6.0917516218721</v>
+        <v>5.9128160418483002</v>
       </c>
       <c r="D5" s="3">
-        <v>6.03985171455051</v>
+        <v>5.93554006968641</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -1948,13 +1948,13 @@
         <v>2018</v>
       </c>
       <c r="B6" s="3">
-        <v>5.4543679843826203</v>
+        <v>5.17507958162801</v>
       </c>
       <c r="C6" s="3">
-        <v>5.9404587603709098</v>
+        <v>5.7492020063839497</v>
       </c>
       <c r="D6" s="3">
-        <v>5.9321620302586604</v>
+        <v>5.7752502274795301</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -1962,13 +1962,13 @@
         <v>2016</v>
       </c>
       <c r="B7" s="3">
-        <v>5.5911572052401803</v>
+        <v>5.3244762391415401</v>
       </c>
       <c r="C7" s="3">
-        <v>5.9224890829694301</v>
+        <v>5.7407975460122698</v>
       </c>
       <c r="D7" s="3">
-        <v>5.9432314410480398</v>
+        <v>5.8065506653019403</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
@@ -1976,13 +1976,13 @@
         <v>2014</v>
       </c>
       <c r="B8" s="3">
-        <v>5.6288271314177996</v>
+        <v>5.3756637168141603</v>
       </c>
       <c r="C8" s="3">
-        <v>6.0089495996231799</v>
+        <v>5.8399822695035501</v>
       </c>
       <c r="D8" s="3">
-        <v>6.06029203956665</v>
+        <v>5.9203539823008899</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -1990,13 +1990,13 @@
         <v>2012</v>
       </c>
       <c r="B9" s="3">
-        <v>5.5086837294332698</v>
+        <v>5.3862038664323402</v>
       </c>
       <c r="C9" s="3">
-        <v>5.8761425959780604</v>
+        <v>5.7861552028218703</v>
       </c>
       <c r="D9" s="3">
-        <v>5.8976234003656298</v>
+        <v>5.8337730870712399</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
@@ -2004,13 +2004,13 @@
         <v>2010</v>
       </c>
       <c r="B10" s="3">
-        <v>5.5307457479284796</v>
+        <v>5.3556935817805398</v>
       </c>
       <c r="C10" s="3">
-        <v>5.7025730484082002</v>
+        <v>5.6193656093489102</v>
       </c>
       <c r="D10" s="3">
-        <v>5.8791975577845603</v>
+        <v>5.7862785862785904</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -2018,13 +2018,13 @@
         <v>2008</v>
       </c>
       <c r="B11" s="3">
-        <v>5.5002255299954896</v>
+        <v>5.2687393526405497</v>
       </c>
       <c r="C11" s="3">
-        <v>5.8304014433919704</v>
+        <v>5.6821870995301103</v>
       </c>
       <c r="D11" s="3">
-        <v>5.7365809652683799</v>
+        <v>5.62079250106519</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
@@ -2032,13 +2032,13 @@
         <v>2006</v>
       </c>
       <c r="B12" s="3">
-        <v>5.6009721608484302</v>
+        <v>5.4035234899328799</v>
       </c>
       <c r="C12" s="3">
-        <v>5.9067609368095404</v>
+        <v>5.7802013422818801</v>
       </c>
       <c r="D12" s="3">
-        <v>5.80247459125055</v>
+        <v>5.6838574423480104</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
@@ -2046,13 +2046,13 @@
         <v>2004</v>
       </c>
       <c r="B13" s="3">
-        <v>5.3431754874651798</v>
+        <v>5.1362916006339203</v>
       </c>
       <c r="C13" s="3">
-        <v>5.6607242339832897</v>
+        <v>5.5459373340414198</v>
       </c>
       <c r="D13" s="3">
-        <v>5.7615598885793897</v>
+        <v>5.6663135593220399</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
@@ -2060,13 +2060,13 @@
         <v>2002</v>
       </c>
       <c r="B14" s="3">
-        <v>5.34383202099737</v>
+        <v>5.0473401659346004</v>
       </c>
       <c r="C14" s="3">
-        <v>5.7406824146981599</v>
+        <v>5.5454545454545396</v>
       </c>
       <c r="D14" s="3">
-        <v>5.58215223097113</v>
+        <v>5.4247311827956999</v>
       </c>
     </row>
   </sheetData>
@@ -2078,9 +2078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBEA1FC-4D97-439E-9D00-72166E73541D}">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -2187,19 +2185,19 @@
         <v>26</v>
       </c>
       <c r="N2">
-        <v>5.7406824146981599</v>
+        <v>5.5454545454545396</v>
       </c>
       <c r="O2">
-        <v>1905</v>
+        <v>2052</v>
       </c>
       <c r="P2">
-        <v>5.6559052779569496</v>
+        <v>5.4538150077266403</v>
       </c>
       <c r="Q2">
-        <v>5.8254595514393799</v>
+        <v>5.6370940831824496</v>
       </c>
       <c r="R2">
-        <v>4.3253641194496303E-2</v>
+        <v>4.6754866187707002E-2</v>
       </c>
       <c r="S2" t="s">
         <v>29</v>
@@ -2249,19 +2247,19 @@
         <v>26</v>
       </c>
       <c r="N3">
-        <v>5.58215223097113</v>
+        <v>5.4247311827956999</v>
       </c>
       <c r="O3">
-        <v>1905</v>
+        <v>2052</v>
       </c>
       <c r="P3">
-        <v>5.4966319114219697</v>
+        <v>5.3347518310843096</v>
       </c>
       <c r="Q3">
-        <v>5.6676725505202903</v>
+        <v>5.5147105345070901</v>
       </c>
       <c r="R3">
-        <v>4.3632816096509597E-2</v>
+        <v>4.5907832505811798E-2</v>
       </c>
       <c r="S3" t="s">
         <v>29</v>
@@ -2311,19 +2309,19 @@
         <v>26</v>
       </c>
       <c r="N4">
-        <v>5.34383202099737</v>
+        <v>5.0473401659346004</v>
       </c>
       <c r="O4">
-        <v>1905</v>
+        <v>2052</v>
       </c>
       <c r="P4">
-        <v>5.2574957549305603</v>
+        <v>4.9513657917123899</v>
       </c>
       <c r="Q4">
-        <v>5.4301682870641796</v>
+        <v>5.1433145401568199</v>
       </c>
       <c r="R4">
-        <v>4.4049115340209499E-2</v>
+        <v>4.8966517460314198E-2</v>
       </c>
       <c r="S4" t="s">
         <v>29</v>
@@ -2373,19 +2371,19 @@
         <v>26</v>
       </c>
       <c r="N5">
-        <v>5.6607242339832897</v>
+        <v>5.5459373340414198</v>
       </c>
       <c r="O5">
-        <v>1795</v>
+        <v>1897</v>
       </c>
       <c r="P5">
-        <v>5.5716533236806498</v>
+        <v>5.4532914123852203</v>
       </c>
       <c r="Q5">
-        <v>5.7497951442859296</v>
+        <v>5.6385832556976201</v>
       </c>
       <c r="R5">
-        <v>4.5444341991142799E-2</v>
+        <v>4.72683273756122E-2</v>
       </c>
       <c r="S5" t="s">
         <v>29</v>
@@ -2435,19 +2433,19 @@
         <v>26</v>
       </c>
       <c r="N6">
-        <v>5.7615598885793897</v>
+        <v>5.6663135593220399</v>
       </c>
       <c r="O6">
-        <v>1795</v>
+        <v>1897</v>
       </c>
       <c r="P6">
-        <v>5.6733938316469201</v>
+        <v>5.5748344607409903</v>
       </c>
       <c r="Q6">
-        <v>5.8497259455118602</v>
+        <v>5.7577926579030798</v>
       </c>
       <c r="R6">
-        <v>4.4982682108403303E-2</v>
+        <v>4.6673009480124102E-2</v>
       </c>
       <c r="S6" t="s">
         <v>29</v>
@@ -2497,19 +2495,19 @@
         <v>26</v>
       </c>
       <c r="N7">
-        <v>5.3431754874651798</v>
+        <v>5.1362916006339203</v>
       </c>
       <c r="O7">
-        <v>1795</v>
+        <v>1897</v>
       </c>
       <c r="P7">
-        <v>5.2520507928693698</v>
+        <v>5.0381822965655099</v>
       </c>
       <c r="Q7">
-        <v>5.4343001820609897</v>
+        <v>5.2344009047023201</v>
       </c>
       <c r="R7">
-        <v>4.64921911203105E-2</v>
+        <v>5.0055767381839103E-2</v>
       </c>
       <c r="S7" t="s">
         <v>29</v>
@@ -2559,19 +2557,19 @@
         <v>26</v>
       </c>
       <c r="N8">
-        <v>5.9067609368095404</v>
+        <v>5.7802013422818801</v>
       </c>
       <c r="O8">
-        <v>2263</v>
+        <v>2394</v>
       </c>
       <c r="P8">
-        <v>5.8290963025940004</v>
+        <v>5.6976388389597199</v>
       </c>
       <c r="Q8">
-        <v>5.9844255710250804</v>
+        <v>5.8627638456040296</v>
       </c>
       <c r="R8">
-        <v>3.9624813375276097E-2</v>
+        <v>4.2123726184772801E-2</v>
       </c>
       <c r="S8" t="s">
         <v>29</v>
@@ -2621,19 +2619,19 @@
         <v>26</v>
       </c>
       <c r="N9">
-        <v>5.80247459125055</v>
+        <v>5.6838574423480104</v>
       </c>
       <c r="O9">
-        <v>2263</v>
+        <v>2394</v>
       </c>
       <c r="P9">
-        <v>5.7248129546277404</v>
+        <v>5.6025661233647099</v>
       </c>
       <c r="Q9">
-        <v>5.8801362278733604</v>
+        <v>5.7651487613313099</v>
       </c>
       <c r="R9">
-        <v>3.9623283991231301E-2</v>
+        <v>4.1475162746580502E-2</v>
       </c>
       <c r="S9" t="s">
         <v>29</v>
@@ -2683,19 +2681,19 @@
         <v>26</v>
       </c>
       <c r="N10">
-        <v>5.6009721608484302</v>
+        <v>5.4035234899328799</v>
       </c>
       <c r="O10">
-        <v>2263</v>
+        <v>2394</v>
       </c>
       <c r="P10">
-        <v>5.5203799726219502</v>
+        <v>5.31647088441989</v>
       </c>
       <c r="Q10">
-        <v>5.6815643490749199</v>
+        <v>5.4905760954458698</v>
       </c>
       <c r="R10">
-        <v>4.1118463380859102E-2</v>
+        <v>4.4414594649484697E-2</v>
       </c>
       <c r="S10" t="s">
         <v>29</v>
@@ -2745,19 +2743,19 @@
         <v>26</v>
       </c>
       <c r="N11">
-        <v>5.8304014433919704</v>
+        <v>5.6821870995301103</v>
       </c>
       <c r="O11">
-        <v>2217</v>
+        <v>2352</v>
       </c>
       <c r="P11">
-        <v>5.7496546459367499</v>
+        <v>5.5965545601090598</v>
       </c>
       <c r="Q11">
-        <v>5.91114824084719</v>
+        <v>5.7678196389511696</v>
       </c>
       <c r="R11">
-        <v>4.11973456404175E-2</v>
+        <v>4.3690071133192801E-2</v>
       </c>
       <c r="S11" t="s">
         <v>29</v>
@@ -2807,19 +2805,19 @@
         <v>26</v>
       </c>
       <c r="N12">
-        <v>5.7365809652683799</v>
+        <v>5.62079250106519</v>
       </c>
       <c r="O12">
-        <v>2217</v>
+        <v>2352</v>
       </c>
       <c r="P12">
-        <v>5.6560866722530099</v>
+        <v>5.5368182596788103</v>
       </c>
       <c r="Q12">
-        <v>5.8170752582837499</v>
+        <v>5.7047667424515698</v>
       </c>
       <c r="R12">
-        <v>4.1068516844576103E-2</v>
+        <v>4.2844000707334601E-2</v>
       </c>
       <c r="S12" t="s">
         <v>29</v>
@@ -2869,19 +2867,19 @@
         <v>26</v>
       </c>
       <c r="N13">
-        <v>5.5002255299954896</v>
+        <v>5.2687393526405497</v>
       </c>
       <c r="O13">
-        <v>2217</v>
+        <v>2352</v>
       </c>
       <c r="P13">
-        <v>5.4167830858875199</v>
+        <v>5.1779302226919004</v>
       </c>
       <c r="Q13">
-        <v>5.5836679741034603</v>
+        <v>5.3595484825891901</v>
       </c>
       <c r="R13">
-        <v>4.2572675565291603E-2</v>
+        <v>4.6331188749307799E-2</v>
       </c>
       <c r="S13" t="s">
         <v>29</v>
@@ -2931,19 +2929,19 @@
         <v>26</v>
       </c>
       <c r="N14">
-        <v>5.7025730484082002</v>
+        <v>5.6193656093489102</v>
       </c>
       <c r="O14">
-        <v>2293</v>
+        <v>2422</v>
       </c>
       <c r="P14">
-        <v>5.6236329116104997</v>
+        <v>5.5378847815901899</v>
       </c>
       <c r="Q14">
-        <v>5.7815131852058999</v>
+        <v>5.7008464371076402</v>
       </c>
       <c r="R14">
-        <v>4.0275579998826597E-2</v>
+        <v>4.1571850897309297E-2</v>
       </c>
       <c r="S14" t="s">
         <v>29</v>
@@ -2993,19 +2991,19 @@
         <v>26</v>
       </c>
       <c r="N15">
-        <v>5.8791975577845603</v>
+        <v>5.7862785862785904</v>
       </c>
       <c r="O15">
-        <v>2293</v>
+        <v>2422</v>
       </c>
       <c r="P15">
-        <v>5.8042356954881003</v>
+        <v>5.7094247806846399</v>
       </c>
       <c r="Q15">
-        <v>5.9541594200810204</v>
+        <v>5.86313239187254</v>
       </c>
       <c r="R15">
-        <v>3.8245848110437297E-2</v>
+        <v>3.9211125303035201E-2</v>
       </c>
       <c r="S15" t="s">
         <v>29</v>
@@ -3055,19 +3053,19 @@
         <v>26</v>
       </c>
       <c r="N16">
-        <v>5.5307457479284796</v>
+        <v>5.3556935817805398</v>
       </c>
       <c r="O16">
-        <v>2293</v>
+        <v>2422</v>
       </c>
       <c r="P16">
-        <v>5.4503016860928799</v>
+        <v>5.2694984210147604</v>
       </c>
       <c r="Q16">
-        <v>5.6111898097640696</v>
+        <v>5.44188874254632</v>
       </c>
       <c r="R16">
-        <v>4.1042888691630502E-2</v>
+        <v>4.3977122839684697E-2</v>
       </c>
       <c r="S16" t="s">
         <v>29</v>
@@ -3117,19 +3115,19 @@
         <v>26</v>
       </c>
       <c r="N17">
-        <v>5.8761425959780604</v>
+        <v>5.7861552028218703</v>
       </c>
       <c r="O17">
-        <v>2188</v>
+        <v>2286</v>
       </c>
       <c r="P17">
-        <v>5.7992877551457704</v>
+        <v>5.70667760163722</v>
       </c>
       <c r="Q17">
-        <v>5.9529974368103602</v>
+        <v>5.8656328040065198</v>
       </c>
       <c r="R17">
-        <v>3.9211653485864702E-2</v>
+        <v>4.05497965227802E-2</v>
       </c>
       <c r="S17" t="s">
         <v>29</v>
@@ -3179,19 +3177,19 @@
         <v>26</v>
       </c>
       <c r="N18">
-        <v>5.8976234003656298</v>
+        <v>5.8337730870712399</v>
       </c>
       <c r="O18">
-        <v>2188</v>
+        <v>2286</v>
       </c>
       <c r="P18">
-        <v>5.8197122561245198</v>
+        <v>5.7540942154058703</v>
       </c>
       <c r="Q18">
-        <v>5.9755345446067398</v>
+        <v>5.9134519587366103</v>
       </c>
       <c r="R18">
-        <v>3.9750583796483697E-2</v>
+        <v>4.06524855435558E-2</v>
       </c>
       <c r="S18" t="s">
         <v>29</v>
@@ -3241,19 +3239,19 @@
         <v>26</v>
       </c>
       <c r="N19">
-        <v>5.5086837294332698</v>
+        <v>5.3862038664323402</v>
       </c>
       <c r="O19">
-        <v>2188</v>
+        <v>2286</v>
       </c>
       <c r="P19">
-        <v>5.4266479176051403</v>
+        <v>5.2996685740229799</v>
       </c>
       <c r="Q19">
-        <v>5.5907195412614001</v>
+        <v>5.4727391588416898</v>
       </c>
       <c r="R19">
-        <v>4.1855006034758897E-2</v>
+        <v>4.4150659392529802E-2</v>
       </c>
       <c r="S19" t="s">
         <v>29</v>
@@ -3303,19 +3301,19 @@
         <v>26</v>
       </c>
       <c r="N20">
-        <v>6.0089495996231799</v>
+        <v>5.8399822695035501</v>
       </c>
       <c r="O20">
-        <v>2123</v>
+        <v>2264</v>
       </c>
       <c r="P20">
-        <v>5.93104704865216</v>
+        <v>5.7552859176087496</v>
       </c>
       <c r="Q20">
-        <v>6.0868521505941899</v>
+        <v>5.92467862139834</v>
       </c>
       <c r="R20">
-        <v>3.9746199475006003E-2</v>
+        <v>4.3212424436121603E-2</v>
       </c>
       <c r="S20" t="s">
         <v>29</v>
@@ -3365,19 +3363,19 @@
         <v>26</v>
       </c>
       <c r="N21">
-        <v>6.06029203956665</v>
+        <v>5.9203539823008899</v>
       </c>
       <c r="O21">
-        <v>2123</v>
+        <v>2264</v>
       </c>
       <c r="P21">
-        <v>5.9802970151463501</v>
+        <v>5.8360152588950802</v>
       </c>
       <c r="Q21">
-        <v>6.1402870639869498</v>
+        <v>6.0046927057066899</v>
       </c>
       <c r="R21">
-        <v>4.0813787969540299E-2</v>
+        <v>4.3029960921327E-2</v>
       </c>
       <c r="S21" t="s">
         <v>29</v>
@@ -3427,19 +3425,19 @@
         <v>26</v>
       </c>
       <c r="N22">
-        <v>5.6288271314177996</v>
+        <v>5.3756637168141603</v>
       </c>
       <c r="O22">
-        <v>2123</v>
+        <v>2264</v>
       </c>
       <c r="P22">
-        <v>5.5466383520923497</v>
+        <v>5.2842870703895501</v>
       </c>
       <c r="Q22">
-        <v>5.7110159107432601</v>
+        <v>5.4670403632387696</v>
       </c>
       <c r="R22">
-        <v>4.1933050676253601E-2</v>
+        <v>4.6620737971741003E-2</v>
       </c>
       <c r="S22" t="s">
         <v>29</v>
@@ -3489,19 +3487,19 @@
         <v>26</v>
       </c>
       <c r="N23">
-        <v>5.9224890829694301</v>
+        <v>5.7407975460122698</v>
       </c>
       <c r="O23">
-        <v>1832</v>
+        <v>1959</v>
       </c>
       <c r="P23">
-        <v>5.8381770020975301</v>
+        <v>5.6495557880663902</v>
       </c>
       <c r="Q23">
-        <v>6.0068011638413301</v>
+        <v>5.8320393039581502</v>
       </c>
       <c r="R23">
-        <v>4.30163677917847E-2</v>
+        <v>4.6551917319327597E-2</v>
       </c>
       <c r="S23" t="s">
         <v>29</v>
@@ -3551,19 +3549,19 @@
         <v>26</v>
       </c>
       <c r="N24">
-        <v>5.9432314410480398</v>
+        <v>5.8065506653019403</v>
       </c>
       <c r="O24">
-        <v>1832</v>
+        <v>1959</v>
       </c>
       <c r="P24">
-        <v>5.8606825670878102</v>
+        <v>5.7193733618865803</v>
       </c>
       <c r="Q24">
-        <v>6.0257803150082596</v>
+        <v>5.8937279687173101</v>
       </c>
       <c r="R24">
-        <v>4.21167724286838E-2</v>
+        <v>4.4478216028247503E-2</v>
       </c>
       <c r="S24" t="s">
         <v>29</v>
@@ -3613,19 +3611,19 @@
         <v>26</v>
       </c>
       <c r="N25">
-        <v>5.5911572052401803</v>
+        <v>5.3244762391415401</v>
       </c>
       <c r="O25">
-        <v>1832</v>
+        <v>1959</v>
       </c>
       <c r="P25">
-        <v>5.5032685227715197</v>
+        <v>5.2266838881319799</v>
       </c>
       <c r="Q25">
-        <v>5.6790458877088303</v>
+        <v>5.4222685901511003</v>
       </c>
       <c r="R25">
-        <v>4.4841164524824798E-2</v>
+        <v>4.9894056637532103E-2</v>
       </c>
       <c r="S25" t="s">
         <v>29</v>
@@ -3675,19 +3673,19 @@
         <v>26</v>
       </c>
       <c r="N26">
-        <v>5.9404587603709098</v>
+        <v>5.7492020063839497</v>
       </c>
       <c r="O26">
-        <v>2049</v>
+        <v>2204</v>
       </c>
       <c r="P26">
-        <v>5.8585603661495202</v>
+        <v>5.6617764785955096</v>
       </c>
       <c r="Q26">
-        <v>6.0223571545923003</v>
+        <v>5.8366275341723899</v>
       </c>
       <c r="R26">
-        <v>4.1784895010913002E-2</v>
+        <v>4.4604861116550799E-2</v>
       </c>
       <c r="S26" t="s">
         <v>29</v>
@@ -3737,19 +3735,19 @@
         <v>26</v>
       </c>
       <c r="N27">
-        <v>5.9321620302586604</v>
+        <v>5.7752502274795301</v>
       </c>
       <c r="O27">
-        <v>2049</v>
+        <v>2204</v>
       </c>
       <c r="P27">
-        <v>5.8511807037635899</v>
+        <v>5.69047387146838</v>
       </c>
       <c r="Q27">
-        <v>6.01314335675373</v>
+        <v>5.8600265834906802</v>
       </c>
       <c r="R27">
-        <v>4.13170033138116E-2</v>
+        <v>4.3253242862831401E-2</v>
       </c>
       <c r="S27" t="s">
         <v>29</v>
@@ -3799,19 +3797,19 @@
         <v>26</v>
       </c>
       <c r="N28">
-        <v>5.4543679843826203</v>
+        <v>5.17507958162801</v>
       </c>
       <c r="O28">
-        <v>2049</v>
+        <v>2204</v>
       </c>
       <c r="P28">
-        <v>5.3673362899802397</v>
+        <v>5.0795520173124897</v>
       </c>
       <c r="Q28">
-        <v>5.5413996787850097</v>
+        <v>5.2706071459435302</v>
       </c>
       <c r="R28">
-        <v>4.44039257155045E-2</v>
+        <v>4.8738553222203801E-2</v>
       </c>
       <c r="S28" t="s">
         <v>29</v>
@@ -3861,19 +3859,19 @@
         <v>26</v>
       </c>
       <c r="N29">
-        <v>6.0917516218721</v>
+        <v>5.9128160418483002</v>
       </c>
       <c r="O29">
-        <v>1079</v>
+        <v>1149</v>
       </c>
       <c r="P29">
-        <v>5.9830158548003602</v>
+        <v>5.7944868591251799</v>
       </c>
       <c r="Q29">
-        <v>6.2004873889438503</v>
+        <v>6.0311452245714197</v>
       </c>
       <c r="R29">
-        <v>5.5477432179461598E-2</v>
+        <v>6.0372032001593197E-2</v>
       </c>
       <c r="S29" t="s">
         <v>29</v>
@@ -3923,19 +3921,19 @@
         <v>26</v>
       </c>
       <c r="N30">
-        <v>6.03985171455051</v>
+        <v>5.93554006968641</v>
       </c>
       <c r="O30">
-        <v>1079</v>
+        <v>1149</v>
       </c>
       <c r="P30">
-        <v>5.9279814454395598</v>
+        <v>5.8187012691138102</v>
       </c>
       <c r="Q30">
-        <v>6.1517219836614601</v>
+        <v>6.0523788702590098</v>
       </c>
       <c r="R30">
-        <v>5.7076667913752502E-2</v>
+        <v>5.96116329452024E-2</v>
       </c>
       <c r="S30" t="s">
         <v>29</v>
@@ -3985,19 +3983,19 @@
         <v>26</v>
       </c>
       <c r="N31">
-        <v>5.7015755329008302</v>
+        <v>5.4255874673629201</v>
       </c>
       <c r="O31">
-        <v>1079</v>
+        <v>1149</v>
       </c>
       <c r="P31">
-        <v>5.5874746057821696</v>
+        <v>5.2970507491747902</v>
       </c>
       <c r="Q31">
-        <v>5.8156764600194997</v>
+        <v>5.5541241855510597</v>
       </c>
       <c r="R31">
-        <v>5.8214758734013501E-2</v>
+        <v>6.5579958259253002E-2</v>
       </c>
       <c r="S31" t="s">
         <v>29</v>

</xml_diff>